<commit_message>
More art, GMG updated
</commit_message>
<xml_diff>
--- a/data/Orcus - Ancestries.xlsx
+++ b/data/Orcus - Ancestries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Obsidian\Tabletop games\d20 System or D&amp;D-esque\2021 Orcus - 4E clone\GitHub\orcus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD883C25-F1C3-4542-868B-2A8D3750661E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E58D209-3D02-4A77-BB9E-D37732BE51CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{395833C3-F072-42E3-B9AA-61F18D49D34E}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="210">
   <si>
     <t>Name</t>
   </si>
@@ -654,6 +654,12 @@
   </si>
   <si>
     <t>7 squares</t>
+  </si>
+  <si>
+    <t>&lt;figure&gt;&lt;img src="pics\DnD_Minotaur.png" alt="Minotaur by LadyofHats" style="zoom: 100%;" /&gt;&lt;figcaption&gt;Minotaur by LadyofHats&lt;/figcaption&gt;&lt;/figure&gt;</t>
+  </si>
+  <si>
+    <t>&lt;figure&gt;&lt;img src="pics\DnD_Nixie.png" alt="Nixie by LadyofHats" style="zoom: 100%;" /&gt;&lt;figcaption&gt;Nixie by LadyofHats&lt;/figcaption&gt;&lt;/figure&gt;</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1018,7 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1384,7 +1390,7 @@
         <v>58</v>
       </c>
       <c r="E8" t="str">
-        <f>LOWER(D8)</f>
+        <f t="shared" ref="E8:E25" si="0">LOWER(D8)</f>
         <v>farstrider</v>
       </c>
       <c r="F8" t="s">
@@ -1441,7 +1447,7 @@
         <v>84</v>
       </c>
       <c r="E9" t="str">
-        <f>LOWER(D9)</f>
+        <f t="shared" si="0"/>
         <v>disappearing act</v>
       </c>
       <c r="F9" t="s">
@@ -1492,7 +1498,7 @@
         <v>96</v>
       </c>
       <c r="E10" t="str">
-        <f>LOWER(D10)</f>
+        <f t="shared" si="0"/>
         <v>violent rush</v>
       </c>
       <c r="F10" t="s">
@@ -1540,7 +1546,7 @@
         <v>15</v>
       </c>
       <c r="E11" t="str">
-        <f>LOWER(D11)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F11" t="s">
@@ -1588,7 +1594,7 @@
         <v>108</v>
       </c>
       <c r="E12" t="str">
-        <f>LOWER(D12)</f>
+        <f t="shared" si="0"/>
         <v>stomp</v>
       </c>
       <c r="F12" t="s">
@@ -1636,7 +1642,7 @@
         <v>114</v>
       </c>
       <c r="E13" t="str">
-        <f>LOWER(D13)</f>
+        <f t="shared" si="0"/>
         <v>careful focus</v>
       </c>
       <c r="F13" t="s">
@@ -1687,7 +1693,7 @@
         <v>127</v>
       </c>
       <c r="E14" t="str">
-        <f>LOWER(D14)</f>
+        <f t="shared" si="0"/>
         <v>breath weapon</v>
       </c>
       <c r="F14" t="s">
@@ -1734,11 +1740,14 @@
       <c r="B15" t="s">
         <v>15</v>
       </c>
+      <c r="C15" t="s">
+        <v>208</v>
+      </c>
       <c r="D15" t="s">
         <v>133</v>
       </c>
       <c r="E15" t="str">
-        <f>LOWER(D15)</f>
+        <f t="shared" si="0"/>
         <v>momentum blow</v>
       </c>
       <c r="F15" t="s">
@@ -1786,7 +1795,7 @@
         <v>141</v>
       </c>
       <c r="E16" t="str">
-        <f>LOWER(D16)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F16" t="s">
@@ -1836,11 +1845,14 @@
       <c r="B17" t="s">
         <v>147</v>
       </c>
+      <c r="C17" t="s">
+        <v>209</v>
+      </c>
       <c r="D17" t="s">
         <v>148</v>
       </c>
       <c r="E17" t="str">
-        <f>LOWER(D17)</f>
+        <f t="shared" si="0"/>
         <v>supernatural beauty</v>
       </c>
       <c r="F17" t="s">
@@ -1888,7 +1900,7 @@
         <v>155</v>
       </c>
       <c r="E18" t="str">
-        <f>LOWER(D18)</f>
+        <f t="shared" si="0"/>
         <v>highblood teleport</v>
       </c>
       <c r="F18" t="s">
@@ -1942,7 +1954,7 @@
         <v>167</v>
       </c>
       <c r="E19" t="str">
-        <f>LOWER(D19)</f>
+        <f t="shared" si="0"/>
         <v>poisonous nip</v>
       </c>
       <c r="F19" t="s">
@@ -1999,7 +2011,7 @@
         <v>68</v>
       </c>
       <c r="E20" t="str">
-        <f>LOWER(D20)</f>
+        <f t="shared" si="0"/>
         <v>sleep dart</v>
       </c>
       <c r="F20" t="s">
@@ -2044,7 +2056,7 @@
         <v>139</v>
       </c>
       <c r="E21" t="str">
-        <f>LOWER(D21)</f>
+        <f t="shared" si="0"/>
         <v>deceptive motion</v>
       </c>
       <c r="F21" t="s">
@@ -2089,7 +2101,7 @@
         <v>44</v>
       </c>
       <c r="E22" t="str">
-        <f>LOWER(D22)</f>
+        <f t="shared" si="0"/>
         <v>vengeance of the pit</v>
       </c>
       <c r="F22" t="s">
@@ -2140,7 +2152,7 @@
         <v>92</v>
       </c>
       <c r="E23" t="str">
-        <f>LOWER(D23)</f>
+        <f t="shared" si="0"/>
         <v>lucky</v>
       </c>
       <c r="F23" t="s">
@@ -2188,7 +2200,7 @@
         <v>121</v>
       </c>
       <c r="E24" t="str">
-        <f>LOWER(D24)</f>
+        <f t="shared" si="0"/>
         <v>travel bug</v>
       </c>
       <c r="F24" t="s">
@@ -2230,7 +2242,7 @@
         <v>75</v>
       </c>
       <c r="E25" t="str">
-        <f>LOWER(D25)</f>
+        <f t="shared" si="0"/>
         <v>blinding mucus</v>
       </c>
       <c r="F25" t="s">

</xml_diff>